<commit_message>
Added some custom functions.
</commit_message>
<xml_diff>
--- a/Input Files/TestData.xlsx
+++ b/Input Files/TestData.xlsx
@@ -5,10 +5,10 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Sharika\Katalon Studio\OrangeHRM\Input Files\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Sharika\git\KatalonProject_OrangeHRM\Input Files\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CB1D0415-2C4E-4D1E-B70A-8EAF7DC57574}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4C3EC059-0651-4418-952B-3CF4D4C734A6}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10300" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -26,7 +26,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="26" uniqueCount="21">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="29" uniqueCount="24">
   <si>
     <t>Username</t>
   </si>
@@ -89,6 +89,15 @@
   </si>
   <si>
     <t>Sachin123</t>
+  </si>
+  <si>
+    <t>Shreyas</t>
+  </si>
+  <si>
+    <t>K</t>
+  </si>
+  <si>
+    <t>Iyer</t>
   </si>
 </sst>
 </file>
@@ -463,10 +472,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{8BBCE071-76B8-4D03-B134-91992CEF9F27}">
-  <dimension ref="A1:D4"/>
+  <dimension ref="A1:D5"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F3" sqref="F3"/>
+      <selection activeCell="D8" sqref="D8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -521,6 +530,17 @@
         <v>20</v>
       </c>
     </row>
+    <row r="5" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A5" t="s">
+        <v>21</v>
+      </c>
+      <c r="B5" t="s">
+        <v>22</v>
+      </c>
+      <c r="C5" t="s">
+        <v>23</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>